<commit_message>
Completed script and RPA for CMACGM
</commit_message>
<xml_diff>
--- a/CMACGM/Test.xlsx
+++ b/CMACGM/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\RPA-Data-Scraping\ShippingStatusTool\APL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blume-proj\OceanCarrierRPA\CMACGM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,175 +57,175 @@
     <t>USG0112045</t>
   </si>
   <si>
+    <t>USG0112868</t>
+  </si>
+  <si>
+    <t>TGBU5076447-USG0112868-IMP</t>
+  </si>
+  <si>
+    <t>TGBU5076447</t>
+  </si>
+  <si>
+    <t>NPMZ006300</t>
+  </si>
+  <si>
+    <t>TCNU8401983-NPMZ006300-IMP</t>
+  </si>
+  <si>
+    <t>TCNU8401983</t>
+  </si>
+  <si>
+    <t>NACH310011</t>
+  </si>
+  <si>
+    <t>TCNU9733540-NACH310011-IMP</t>
+  </si>
+  <si>
+    <t>TCNU9733540</t>
+  </si>
+  <si>
+    <t>SHCT006031</t>
+  </si>
+  <si>
+    <t>TCNU7488736-SHCT006031-IMP</t>
+  </si>
+  <si>
+    <t>TCNU7488736</t>
+  </si>
+  <si>
+    <t>SHKN002182</t>
+  </si>
+  <si>
+    <t>CMAU4650333-SHKN002182-RET</t>
+  </si>
+  <si>
+    <t>CMAU4650333</t>
+  </si>
+  <si>
+    <t>TTGS101995</t>
+  </si>
+  <si>
+    <t>CMAU4568760-TTGS101995-RET</t>
+  </si>
+  <si>
+    <t>CMAU4568760</t>
+  </si>
+  <si>
+    <t>BBI0118658</t>
+  </si>
+  <si>
+    <t>TCNU1113780-BBI0118658-IMP</t>
+  </si>
+  <si>
+    <t>TCNU1113780</t>
+  </si>
+  <si>
+    <t>BBI0118277</t>
+  </si>
+  <si>
+    <t>TCLU1873337-BBI0118277-IMP</t>
+  </si>
+  <si>
+    <t>TCLU1873337</t>
+  </si>
+  <si>
+    <t>SHPE003566</t>
+  </si>
+  <si>
+    <t>TCLU1871709-SHPE003566-IMP</t>
+  </si>
+  <si>
+    <t>TCLU1871709</t>
+  </si>
+  <si>
+    <t>NAZY360034</t>
+  </si>
+  <si>
+    <t>CMAU4196581-NAZY360034-RET</t>
+  </si>
+  <si>
+    <t>CMAU4196581</t>
+  </si>
+  <si>
+    <t>USG0112382</t>
+  </si>
+  <si>
+    <t>TCLU1861038-USG0112382-IMP</t>
+  </si>
+  <si>
+    <t>TCLU1861038</t>
+  </si>
+  <si>
+    <t>SHSS001804</t>
+  </si>
+  <si>
+    <t>GLDU7654220-SHSS001804-IMP</t>
+  </si>
+  <si>
+    <t>GLDU7654220</t>
+  </si>
+  <si>
+    <t>SHPE003572</t>
+  </si>
+  <si>
+    <t>CMAU4095523-SHPE003572-RET</t>
+  </si>
+  <si>
+    <t>CMAU4095523</t>
+  </si>
+  <si>
+    <t>AXK0131826</t>
+  </si>
+  <si>
+    <t>CMAU0838220-AXK0131826-RET</t>
+  </si>
+  <si>
+    <t>CMAU0838220</t>
+  </si>
+  <si>
+    <t>TTWE002802</t>
+  </si>
+  <si>
+    <t>GESU5827758-TTWE002802-IMP</t>
+  </si>
+  <si>
+    <t>GESU5827758</t>
+  </si>
+  <si>
+    <t>BBI0118282</t>
+  </si>
+  <si>
+    <t>APHU7231878-BBI0118282-RET</t>
+  </si>
+  <si>
+    <t>APHU7231878</t>
+  </si>
+  <si>
+    <t>NAZC360170</t>
+  </si>
+  <si>
+    <t>BEAU4046769-NAZC360170-RET</t>
+  </si>
+  <si>
+    <t>BEAU4046769</t>
+  </si>
+  <si>
+    <t>BBI0116890</t>
+  </si>
+  <si>
+    <t>TCNU5514760-BBI0116890-IMP</t>
+  </si>
+  <si>
+    <t>TCNU5514760</t>
+  </si>
+  <si>
+    <t>NPDN008117</t>
+  </si>
+  <si>
+    <t>CMAU5601122-NPDN008117-IMP</t>
+  </si>
+  <si>
     <t>CMAU5601122</t>
-  </si>
-  <si>
-    <t>CMAU5601122-NPDN008117-IMP</t>
-  </si>
-  <si>
-    <t>NPDN008117</t>
-  </si>
-  <si>
-    <t>TCNU5514760</t>
-  </si>
-  <si>
-    <t>TCNU5514760-BBI0116890-IMP</t>
-  </si>
-  <si>
-    <t>BBI0116890</t>
-  </si>
-  <si>
-    <t>BEAU4046769</t>
-  </si>
-  <si>
-    <t>BEAU4046769-NAZC360170-RET</t>
-  </si>
-  <si>
-    <t>NAZC360170</t>
-  </si>
-  <si>
-    <t>APHU7231878</t>
-  </si>
-  <si>
-    <t>APHU7231878-BBI0118282-RET</t>
-  </si>
-  <si>
-    <t>BBI0118282</t>
-  </si>
-  <si>
-    <t>GESU5827758</t>
-  </si>
-  <si>
-    <t>GESU5827758-TTWE002802-IMP</t>
-  </si>
-  <si>
-    <t>TTWE002802</t>
-  </si>
-  <si>
-    <t>CMAU0838220</t>
-  </si>
-  <si>
-    <t>CMAU0838220-AXK0131826-RET</t>
-  </si>
-  <si>
-    <t>AXK0131826</t>
-  </si>
-  <si>
-    <t>CMAU4095523</t>
-  </si>
-  <si>
-    <t>CMAU4095523-SHPE003572-RET</t>
-  </si>
-  <si>
-    <t>SHPE003572</t>
-  </si>
-  <si>
-    <t>GLDU7654220</t>
-  </si>
-  <si>
-    <t>GLDU7654220-SHSS001804-IMP</t>
-  </si>
-  <si>
-    <t>SHSS001804</t>
-  </si>
-  <si>
-    <t>TCLU1861038</t>
-  </si>
-  <si>
-    <t>TCLU1861038-USG0112382-IMP</t>
-  </si>
-  <si>
-    <t>USG0112382</t>
-  </si>
-  <si>
-    <t>CMAU4196581</t>
-  </si>
-  <si>
-    <t>CMAU4196581-NAZY360034-RET</t>
-  </si>
-  <si>
-    <t>NAZY360034</t>
-  </si>
-  <si>
-    <t>TCLU1871709</t>
-  </si>
-  <si>
-    <t>TCLU1871709-SHPE003566-IMP</t>
-  </si>
-  <si>
-    <t>SHPE003566</t>
-  </si>
-  <si>
-    <t>TCLU1873337</t>
-  </si>
-  <si>
-    <t>TCLU1873337-BBI0118277-IMP</t>
-  </si>
-  <si>
-    <t>BBI0118277</t>
-  </si>
-  <si>
-    <t>TCNU1113780</t>
-  </si>
-  <si>
-    <t>TCNU1113780-BBI0118658-IMP</t>
-  </si>
-  <si>
-    <t>BBI0118658</t>
-  </si>
-  <si>
-    <t>CMAU4568760</t>
-  </si>
-  <si>
-    <t>CMAU4568760-TTGS101995-RET</t>
-  </si>
-  <si>
-    <t>TTGS101995</t>
-  </si>
-  <si>
-    <t>CMAU4650333</t>
-  </si>
-  <si>
-    <t>CMAU4650333-SHKN002182-RET</t>
-  </si>
-  <si>
-    <t>SHKN002182</t>
-  </si>
-  <si>
-    <t>TCNU7488736</t>
-  </si>
-  <si>
-    <t>TCNU7488736-SHCT006031-IMP</t>
-  </si>
-  <si>
-    <t>SHCT006031</t>
-  </si>
-  <si>
-    <t>TCNU9733540</t>
-  </si>
-  <si>
-    <t>TCNU9733540-NACH310011-IMP</t>
-  </si>
-  <si>
-    <t>NACH310011</t>
-  </si>
-  <si>
-    <t>TCNU8401983</t>
-  </si>
-  <si>
-    <t>TCNU8401983-NPMZ006300-IMP</t>
-  </si>
-  <si>
-    <t>NPMZ006300</t>
-  </si>
-  <si>
-    <t>TGBU5076447</t>
-  </si>
-  <si>
-    <t>TGBU5076447-USG0112868-IMP</t>
-  </si>
-  <si>
-    <t>USG0112868</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F21"/>
+      <selection activeCell="A3" sqref="A3:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -602,18 +602,18 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -622,18 +622,18 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -642,18 +642,18 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -662,18 +662,18 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -682,18 +682,18 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -702,18 +702,18 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -722,18 +722,18 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -742,18 +742,18 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -762,18 +762,18 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -788,12 +788,12 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -802,18 +802,18 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -822,18 +822,18 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -842,18 +842,18 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -862,18 +862,18 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -882,18 +882,18 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -902,18 +902,18 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -922,18 +922,18 @@
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -942,18 +942,18 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -962,13 +962,13 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>